<commit_message>
Added further tests; updated symbol parser for extended 32-bit registers
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -296,7 +296,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -463,16 +463,19 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
Added all 64-bit MOV register-register tests
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -443,6 +443,7 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -481,16 +482,19 @@
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -538,11 +542,13 @@
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">

</xml_diff>

<commit_message>
Added initial memory tests for mov/r32/er32
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -579,6 +579,7 @@
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -629,11 +630,13 @@
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">

</xml_diff>

<commit_message>
Added add r32 tests (all variants, no imm, mem)
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -421,7 +421,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="0"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
@@ -465,18 +465,21 @@
         <v>12</v>
       </c>
       <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
Added sub r32 tests (all variants, no imm, mem)
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -422,7 +422,7 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="0"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
@@ -466,6 +466,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -473,6 +474,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -480,6 +482,7 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
Added and/or/xor basic r32 register tests
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -423,9 +423,9 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
@@ -467,6 +467,9 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -475,6 +478,9 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -483,6 +489,9 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
Added 64-bit register add variants and tests
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -444,6 +444,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -498,18 +499,21 @@
         <v>15</v>
       </c>
       <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -553,18 +557,21 @@
         <v>25</v>
       </c>
       <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">

</xml_diff>

<commit_message>
Added full register-register/imm support for 16-bit registers
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,6 +460,7 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -534,16 +535,19 @@
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -598,6 +602,7 @@
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">

</xml_diff>

<commit_message>
Added remaining variants for register-register move instructions
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -450,11 +450,13 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -520,16 +522,19 @@
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -587,11 +592,13 @@
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">

</xml_diff>

<commit_message>
Added mem->register for moves (all variants)
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -383,8 +383,8 @@
   </sheetPr>
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,36 +679,43 @@
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="B44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="B46" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added register-to-memory moves; all non-offset moves complete
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -383,8 +383,8 @@
   </sheetPr>
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,46 +622,55 @@
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="B32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">

</xml_diff>

<commit_message>
Added all register-register variants and some register-imm of add/and/or/xor/sub
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,24 +445,43 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -503,6 +522,10 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -510,6 +533,10 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -517,42 +544,76 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -560,6 +621,10 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -567,6 +632,10 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -574,6 +643,10 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -581,6 +654,10 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">

</xml_diff>

<commit_message>
Added remaining register-imm versions for add/and/or/xor/sub
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -664,30 +664,55 @@
         <v>28</v>
       </c>
       <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">

</xml_diff>